<commit_message>
V1.1 Update owner status to closed
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_ADMINCONSTRAINS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_ADMINCONSTRAINS_REVIEWS.xlsx
@@ -1,22 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA122DA8-8C45-48C0-A64E-05DCC449638A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="8832" windowHeight="12336" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="8835" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Version History" sheetId="1" r:id="rId1"/>
-    <sheet name="LH-TC-ADMINCONSTRAINS-Review" sheetId="2" r:id="rId2"/>
+    <sheet name="LH-TC-ADMINCONSTRAINS-Review" sheetId="2" r:id="rId1"/>
+    <sheet name="Version History" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
   <si>
     <t>Author</t>
   </si>
@@ -89,9 +83,6 @@
   </si>
   <si>
     <t>Eman</t>
-  </si>
-  <si>
-    <t>Open</t>
   </si>
   <si>
     <t>SRS-ADM-002 &amp; SRS-ADM-003</t>
@@ -126,12 +117,21 @@
   </si>
   <si>
     <t>Initial version</t>
+  </si>
+  <si>
+    <t>Closed</t>
+  </si>
+  <si>
+    <t>Update owner status to closed</t>
+  </si>
+  <si>
+    <t>v1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -233,44 +233,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="16"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -536,6 +498,44 @@
       </border>
     </dxf>
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="16"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -568,34 +568,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Date" dataDxfId="12">
-      <calculatedColumnFormula>DATE(2025,4,21)</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+  <tableColumns count="10">
+    <tableColumn id="1" name="Date" dataDxfId="9">
+      <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
+    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
+    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
+    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
+    <tableColumn id="4" name="Version" dataDxfId="5"/>
+    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
+    <tableColumn id="6" name="Actions" dataDxfId="3"/>
+    <tableColumn id="7" name="Owner" dataDxfId="2"/>
+    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
+    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Date" dataDxfId="11">
-      <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+  <tableColumns count="4">
+    <tableColumn id="1" name="Version Number" dataDxfId="15"/>
+    <tableColumn id="2" name="Author" dataDxfId="14"/>
+    <tableColumn id="3" name="Updated Section" dataDxfId="13"/>
+    <tableColumn id="4" name="Date" dataDxfId="12">
+      <calculatedColumnFormula>DATE(2025,4,21)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0100-00000B000000}" name="Review ID" dataDxfId="10"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Reviewed Entity" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Reviewer" dataDxfId="8"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Version" dataDxfId="7"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="Review Comments" dataDxfId="6"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0100-000006000000}" name="Actions" dataDxfId="5"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0100-000007000000}" name="Owner" dataDxfId="4"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0100-000008000000}" name="Owner Status" dataDxfId="3"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0100-000009000000}" name="Reviewer verification" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -890,100 +890,192 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView zoomScale="52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="39.85546875" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
-    <col min="4" max="4" width="11" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" style="7" customWidth="1"/>
+    <col min="3" max="4" width="39.85546875" style="7"/>
+    <col min="5" max="5" width="17.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="86.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="79.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="39.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B2" s="3" t="s">
+      <c r="B1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" s="7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="6">
+        <f t="shared" ref="A2:A4" ca="1" si="0">TODAY()</f>
+        <v>45769</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="D2" s="4">
-        <f t="shared" ref="D2:D9" si="0">DATE(2025,4,21)</f>
-        <v>45768</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-    </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="3"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3"/>
-      <c r="B9" s="3"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
+    </row>
+    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.25">
+      <c r="A3" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45769</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="H3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="A4" s="6">
+        <f t="shared" ca="1" si="0"/>
+        <v>45769</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576">
+      <formula1>"open,inProgress,notApplicable,close"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12">
+      <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12">
+      <formula1>"Open,Closed"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -992,185 +1084,102 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:J12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39.88671875" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="54.109375" style="7" customWidth="1"/>
-    <col min="3" max="4" width="39.88671875" style="7"/>
-    <col min="5" max="5" width="17.5546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="86.33203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="79.77734375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="26.109375" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="39.88671875" style="7"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="D1" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" s="7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" s="7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" s="7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="6">
-        <f t="shared" ref="A2:A12" ca="1" si="0">TODAY()</f>
+    </row>
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="4">
+        <f t="shared" ref="D2:D3" si="0">DATE(2025,4,21)</f>
+        <v>45768</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="4">
+        <f>DATE(2025,4,22)</f>
         <v>45769</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="H2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I2" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.3">
-      <c r="A3" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45769</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="G3" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I3" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.3">
-      <c r="A4" s="6">
-        <f t="shared" ca="1" si="0"/>
-        <v>45769</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="I4" s="7" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="6"/>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="3"/>
+      <c r="D4" s="4"/>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="4"/>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="4"/>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="4"/>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="4"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0100-000000000000}">
-      <formula1>"open,inProgress,notApplicable,close"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12" xr:uid="{00000000-0002-0000-0100-000001000000}">
-      <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12" xr:uid="{00000000-0002-0000-0100-000002000000}">
-      <formula1>"Open,Closed"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
v1.2 The comments closed
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_ADMINCONSTRAINS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_ADMINCONSTRAINS_REVIEWS.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27B0FB1-842D-4E7A-BBC2-C5A8D98A650B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-90" yWindow="0" windowWidth="8835" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LH-TC-ADMINCONSTRAINS-Review" sheetId="2" r:id="rId1"/>
     <sheet name="Version History" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -29,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
   <si>
     <t>Author</t>
   </si>
@@ -126,12 +132,18 @@
   </si>
   <si>
     <t>v1.1</t>
+  </si>
+  <si>
+    <t>v1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The comments closed </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -221,6 +233,25 @@
   </cellStyles>
   <dxfs count="18">
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <strike val="0"/>
         <outline val="0"/>
@@ -535,25 +566,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -568,32 +580,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="10">
-    <tableColumn id="1" name="Date" dataDxfId="9">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="15">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" name="Review ID" dataDxfId="8"/>
-    <tableColumn id="2" name="Reviewed Entity" dataDxfId="7"/>
-    <tableColumn id="3" name="Reviewer" dataDxfId="6"/>
-    <tableColumn id="4" name="Version" dataDxfId="5"/>
-    <tableColumn id="5" name="Review Comments" dataDxfId="4"/>
-    <tableColumn id="6" name="Actions" dataDxfId="3"/>
-    <tableColumn id="7" name="Owner" dataDxfId="2"/>
-    <tableColumn id="8" name="Owner Status" dataDxfId="1"/>
-    <tableColumn id="9" name="Reviewer verification" dataDxfId="0"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Review ID" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Reviewed Entity" dataDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Reviewer" dataDxfId="12"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Version" dataDxfId="11"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Review Comments" dataDxfId="10"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Actions" dataDxfId="9"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Owner" dataDxfId="8"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Owner Status" dataDxfId="7"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Reviewer verification" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" name="Version Number" dataDxfId="15"/>
-    <tableColumn id="2" name="Author" dataDxfId="14"/>
-    <tableColumn id="3" name="Updated Section" dataDxfId="13"/>
-    <tableColumn id="4" name="Date" dataDxfId="12">
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Version Number" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Author" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Updated Section" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date" dataDxfId="0">
       <calculatedColumnFormula>DATE(2025,4,21)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -890,34 +902,34 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J12"/>
   <sheetViews>
-    <sheetView zoomScale="52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView topLeftCell="C1" zoomScale="52" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39.85546875" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="39.88671875" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.5703125" style="7" customWidth="1"/>
-    <col min="2" max="2" width="54.140625" style="7" customWidth="1"/>
-    <col min="3" max="4" width="39.85546875" style="7"/>
-    <col min="5" max="5" width="17.5703125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="86.28515625" style="7" customWidth="1"/>
-    <col min="7" max="7" width="79.7109375" style="7" customWidth="1"/>
-    <col min="8" max="8" width="28.28515625" style="7" customWidth="1"/>
-    <col min="9" max="9" width="26.140625" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="39.85546875" style="7"/>
+    <col min="1" max="1" width="28.5546875" style="7" customWidth="1"/>
+    <col min="2" max="2" width="54.109375" style="7" customWidth="1"/>
+    <col min="3" max="4" width="39.88671875" style="7"/>
+    <col min="5" max="5" width="17.5546875" style="7" customWidth="1"/>
+    <col min="6" max="6" width="86.33203125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="79.6640625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="28.33203125" style="7" customWidth="1"/>
+    <col min="9" max="9" width="26.109375" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="39.88671875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -949,7 +961,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6">
         <f t="shared" ref="A2:A4" ca="1" si="0">TODAY()</f>
         <v>45769</v>
@@ -978,8 +990,11 @@
       <c r="I2" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.25">
+      <c r="J2" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.3">
       <c r="A3" s="6">
         <f t="shared" ca="1" si="0"/>
         <v>45769</v>
@@ -1008,8 +1023,11 @@
       <c r="I3" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+      <c r="J3" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.3">
       <c r="A4" s="6">
         <f t="shared" ca="1" si="0"/>
         <v>45769</v>
@@ -1038,41 +1056,44 @@
       <c r="I4" s="7" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J4" s="7" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1084,22 +1105,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="36.5703125" customWidth="1"/>
+    <col min="1" max="1" width="25.109375" customWidth="1"/>
+    <col min="2" max="2" width="14.5546875" customWidth="1"/>
+    <col min="3" max="3" width="36.5546875" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1113,7 +1134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1124,11 +1145,11 @@
         <v>28</v>
       </c>
       <c r="D2" s="4">
-        <f t="shared" ref="D2:D3" si="0">DATE(2025,4,21)</f>
+        <f t="shared" ref="D2" si="0">DATE(2025,4,21)</f>
         <v>45768</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -1143,43 +1164,53 @@
         <v>45769</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-    </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" s="4">
+        <f>DATE(2025,4,22)</f>
+        <v>45769</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3"/>
       <c r="B5" s="3"/>
       <c r="C5" s="3"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
       <c r="D9" s="4"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>

</xml_diff>

<commit_message>
Baseline LH_REVIEWS Folder from dev branch
</commit_message>
<xml_diff>
--- a/LH_REVIEWS/LH_TC_ADMINCONSTRAINS_REVIEWS.xlsx
+++ b/LH_REVIEWS/LH_TC_ADMINCONSTRAINS_REVIEWS.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\omars\Documents\GitHub\Group-3-Learning-hub\LH_REVIEWS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\halae\OneDrive\Desktop\oooo\Group-3-Learning-hub-dev\LH_REVIEWS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27B0FB1-842D-4E7A-BBC2-C5A8D98A650B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="LH-TC-ADMINCONSTRAINS-Review" sheetId="2" r:id="rId1"/>
     <sheet name="Version History" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="37">
   <si>
     <t>Author</t>
   </si>
@@ -138,12 +137,21 @@
   </si>
   <si>
     <t xml:space="preserve">The comments closed </t>
+  </si>
+  <si>
+    <t>v2.0</t>
+  </si>
+  <si>
+    <t>Hala Eldaly</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Review DELETPOST And No Comments </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -580,32 +588,32 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J12" totalsRowShown="0" headerRowDxfId="17" dataDxfId="16">
   <tableColumns count="10">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Date" dataDxfId="15">
+    <tableColumn id="1" name="Date" dataDxfId="15">
       <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="Review ID" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Reviewed Entity" dataDxfId="13"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Reviewer" dataDxfId="12"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Version" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Review Comments" dataDxfId="10"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Actions" dataDxfId="9"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Owner" dataDxfId="8"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Owner Status" dataDxfId="7"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Reviewer verification" dataDxfId="6"/>
+    <tableColumn id="11" name="Review ID" dataDxfId="14"/>
+    <tableColumn id="2" name="Reviewed Entity" dataDxfId="13"/>
+    <tableColumn id="3" name="Reviewer" dataDxfId="12"/>
+    <tableColumn id="4" name="Version" dataDxfId="11"/>
+    <tableColumn id="5" name="Review Comments" dataDxfId="10"/>
+    <tableColumn id="6" name="Actions" dataDxfId="9"/>
+    <tableColumn id="7" name="Owner" dataDxfId="8"/>
+    <tableColumn id="8" name="Owner Status" dataDxfId="7"/>
+    <tableColumn id="9" name="Reviewer verification" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D9" totalsRowShown="0" headerRowDxfId="5" dataDxfId="4">
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Version Number" dataDxfId="3"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="Author" dataDxfId="2"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Updated Section" dataDxfId="1"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Date" dataDxfId="0">
+    <tableColumn id="1" name="Version Number" dataDxfId="3"/>
+    <tableColumn id="2" name="Author" dataDxfId="2"/>
+    <tableColumn id="3" name="Updated Section" dataDxfId="1"/>
+    <tableColumn id="4" name="Date" dataDxfId="0">
       <calculatedColumnFormula>DATE(2025,4,21)</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -909,27 +917,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScale="52" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="39.88671875" defaultRowHeight="21" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="39.85546875" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.5546875" style="7" customWidth="1"/>
-    <col min="2" max="2" width="54.109375" style="7" customWidth="1"/>
-    <col min="3" max="4" width="39.88671875" style="7"/>
-    <col min="5" max="5" width="17.5546875" style="7" customWidth="1"/>
-    <col min="6" max="6" width="86.33203125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="79.6640625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="28.33203125" style="7" customWidth="1"/>
-    <col min="9" max="9" width="26.109375" style="7" customWidth="1"/>
-    <col min="10" max="16384" width="39.88671875" style="7"/>
+    <col min="1" max="1" width="28.5703125" style="7" customWidth="1"/>
+    <col min="2" max="2" width="54.140625" style="7" customWidth="1"/>
+    <col min="3" max="4" width="39.85546875" style="7"/>
+    <col min="5" max="5" width="17.5703125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="86.28515625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="79.7109375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="26.140625" style="7" customWidth="1"/>
+    <col min="10" max="16384" width="39.85546875" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>1</v>
       </c>
@@ -961,10 +969,10 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <f t="shared" ref="A2:A4" ca="1" si="0">TODAY()</f>
-        <v>45769</v>
+        <v>45790</v>
       </c>
       <c r="B2" s="7" t="s">
         <v>16</v>
@@ -994,10 +1002,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="84" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45769</v>
+        <v>45790</v>
       </c>
       <c r="B3" s="7" t="s">
         <v>21</v>
@@ -1027,10 +1035,10 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <f t="shared" ca="1" si="0"/>
-        <v>45769</v>
+        <v>45790</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>23</v>
@@ -1060,40 +1068,40 @@
         <v>29</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="6"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H13:H1048576">
       <formula1>"open,inProgress,notApplicable,close"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I12">
       <formula1>"Open,InProgress,NotApplicable,Closed"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J12">
       <formula1>"Open,Closed"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1105,22 +1113,22 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C16" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5546875" customWidth="1"/>
-    <col min="3" max="3" width="36.5546875" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.5703125" customWidth="1"/>
+    <col min="3" max="3" width="36.5703125" customWidth="1"/>
     <col min="4" max="4" width="11" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
@@ -1134,7 +1142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1149,7 +1157,7 @@
         <v>45768</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>31</v>
       </c>
@@ -1164,7 +1172,7 @@
         <v>45769</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>32</v>
       </c>
@@ -1179,31 +1187,39 @@
         <v>45769</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D5" s="4">
+        <v>45790</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3"/>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>

</xml_diff>